<commit_message>
seeder, fix input survey
</commit_message>
<xml_diff>
--- a/kito/public/addSurvey.xlsx
+++ b/kito/public/addSurvey.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mag\project mitra\MitraBPS\ProjekMitraBPS\kito\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7190"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19150" windowHeight="2230"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -44,12 +44,6 @@
     <t>kode_kecamatan</t>
   </si>
   <si>
-    <t>kode_kabupaten</t>
-  </si>
-  <si>
-    <t>kode_provinsi</t>
-  </si>
-  <si>
     <t>nama_survei</t>
   </si>
   <si>
@@ -57,6 +51,12 @@
   </si>
   <si>
     <t>contoh</t>
+  </si>
+  <si>
+    <t>KC001</t>
+  </si>
+  <si>
+    <t>D001</t>
   </si>
 </sst>
 </file>
@@ -94,7 +94,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -375,68 +375,63 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="5" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="3" width="8.7265625" style="1"/>
+    <col min="4" max="5" width="10.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" t="s">
-        <v>0</v>
-      </c>
-      <c r="H1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I1" t="s">
-        <v>2</v>
-      </c>
-      <c r="V1" s="1"/>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="G2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H2" s="1" t="s">
+      <c r="E2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I2" t="s">
-        <v>10</v>
+      <c r="G2" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
excel add survei done, update seeder dan table
</commit_message>
<xml_diff>
--- a/kito/public/addSurvey.xlsx
+++ b/kito/public/addSurvey.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RIZKY\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71361830-2CAC-4E98-BB72-B988D0C3CA04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19150" windowHeight="2230"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>kro</t>
   </si>
@@ -57,12 +58,15 @@
   </si>
   <si>
     <t>D001</t>
+  </si>
+  <si>
+    <t>jadwal_berakhir</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -94,7 +98,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -374,63 +378,68 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="8.7265625" style="1"/>
-    <col min="4" max="5" width="10.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.7265625" style="1"/>
+    <col min="4" max="5" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="1">
+        <v>47455</v>
+      </c>
+      <c r="H2" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>